<commit_message>
feat: replace malloc to allocating_only for dynamic tls array#2
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/dynamic_tls.xlsx
+++ b/libalconcurrent/doc/dynamic_tls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_dev\alpha_concurrent\libalconcurrent\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D86B1A-64D1-4157-9D8B-D018A30164B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4412F4-0582-41AE-A8D4-09C811248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="4">
   <si>
     <t>dynamic_tls_key</t>
   </si>
@@ -1446,7 +1446,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>スレッドのライフサイクルに合わせて生成破棄、</a:t>
+            <a:t>スレッドのライフサイクルに合わせて生成</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
@@ -1454,7 +1454,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>or </a:t>
+            <a:t>/</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
@@ -1462,7 +1462,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>生成</a:t>
+            <a:t>無効化</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
@@ -1478,344 +1478,12 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>無効化</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
             <a:t>再利用</a:t>
           </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>209549</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="正方形/長方形 26">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B8768EC-C83E-58AB-42E6-7B8D4DF3B251}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8629650" y="2590799"/>
-          <a:ext cx="2676525" cy="8134351"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>スレッドのライフサイクルに合わせて生成破棄、</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>or </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>生成</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>無効化</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>再利用</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>190501</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="正方形/長方形 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CBF6015-C8A8-4E36-ACC9-24255D4D9419}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5295900" y="895350"/>
-          <a:ext cx="2676525" cy="1438276"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>スレッドのライフサイクルに合わせて生成</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>無効化</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>再利用。破棄はしない。</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>219076</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="正方形/長方形 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B0A8FB-4639-1B85-58B0-0BA11A284DD0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8620125" y="923925"/>
-          <a:ext cx="2676525" cy="1438276"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>スレッドのライフサイクルに合わせて生成</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>無効化</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>/</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>再利用</a:t>
-          </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:effectLst/>
               <a:latin typeface="+mn-lt"/>
@@ -1836,23 +1504,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>209549</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="正方形/長方形 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3EE79FA-B39A-4308-8054-A9E12932CB2C}"/>
+        <xdr:cNvPr id="27" name="正方形/長方形 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B8768EC-C83E-58AB-42E6-7B8D4DF3B251}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1860,7 +1528,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1524000" y="2457449"/>
+          <a:off x="8629650" y="2590799"/>
           <a:ext cx="2676525" cy="8134351"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1890,12 +1558,20 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>スレッドのライフサイクルに合わせて生成</a:t>
+          </a:r>
+          <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>TLS</a:t>
+            <a:t>/</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
@@ -1903,7 +1579,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>の確保要求に従って、動的に追加。領域の</a:t>
+            <a:t>無効化</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
@@ -1911,7 +1587,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>free</a:t>
+            <a:t>/</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
@@ -1919,24 +1595,25 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>はしない。</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>TLS</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>解放後は再利用する。</a:t>
-          </a:r>
+            <a:t>再利用</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>。破棄はしない。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1944,23 +1621,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="正方形/長方形 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17C11CEA-8AE1-4C75-3C36-A4E51AF88EC1}"/>
+        <xdr:cNvPr id="28" name="正方形/長方形 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CBF6015-C8A8-4E36-ACC9-24255D4D9419}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1968,12 +1645,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4676774" y="333375"/>
-          <a:ext cx="2238375" cy="476250"/>
+          <a:off x="5295900" y="895350"/>
+          <a:ext cx="2676525" cy="1438276"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -1997,6 +1675,330 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>スレッドのライフサイクルに合わせて生成</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>無効化</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>再利用。破棄はしない。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>219076</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="正方形/長方形 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B0A8FB-4639-1B85-58B0-0BA11A284DD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8620125" y="923925"/>
+          <a:ext cx="2676525" cy="1438276"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>スレッドのライフサイクルに合わせて生成</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>無効化</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>再利用</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>。破棄はしない。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="正方形/長方形 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3EE79FA-B39A-4308-8054-A9E12932CB2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="2457449"/>
+          <a:ext cx="2676525" cy="8134351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>TLS</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>の確保要求に従って、動的に追加。領域の</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>free</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>はしない。</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>TLS</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>解放後は再利用する。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="正方形/長方形 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17C11CEA-8AE1-4C75-3C36-A4E51AF88EC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4676774" y="333375"/>
+          <a:ext cx="2238375" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
             <a:t>pthread_getspecific()</a:t>
           </a:r>
@@ -2104,6 +2106,438 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="直線矢印コネクタ 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F13F57A7-211D-BA02-9023-AAD8BCD92A75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4000500" y="4905375"/>
+          <a:ext cx="2133600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="直線矢印コネクタ 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE8B68CB-3661-46FA-9094-1E9E961B52FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7696200" y="4895850"/>
+          <a:ext cx="1838325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直線矢印コネクタ 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB1A8E6A-B260-4019-AA26-442141049F0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3990975" y="5133975"/>
+          <a:ext cx="2133600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="直線矢印コネクタ 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83CAB90F-C794-44C8-8379-C618F5580AE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7686675" y="5124450"/>
+          <a:ext cx="1838325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="直線矢印コネクタ 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10535C10-AF68-48CC-93D1-3347E43AEE07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3962400" y="5372100"/>
+          <a:ext cx="2133600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="直線矢印コネクタ 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE246D3B-08D0-4C60-AF56-BCE9F1D53236}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7658100" y="5362575"/>
+          <a:ext cx="1838325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="直線矢印コネクタ 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F760E52A-1ACD-47C4-BFFA-533A5D462A82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3971925" y="5619750"/>
+          <a:ext cx="2133600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="直線矢印コネクタ 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B087EAA-81FB-4247-B0C2-01E0A8EF3492}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7667625" y="5610225"/>
+          <a:ext cx="1838325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -2378,95 +2812,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E21:J48"/>
+  <dimension ref="E21:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData>
-    <row r="21" spans="5:10">
+    <row r="21" spans="5:15">
       <c r="E21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O21" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="22" spans="5:10">
+    <row r="22" spans="5:15">
       <c r="E22" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O22" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="5:15">
       <c r="E23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O23" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="5:15">
       <c r="E24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O24" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="5:15">
       <c r="E25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O25" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="5:15">
       <c r="E26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O26" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="5:15">
       <c r="E27" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="5:15">
       <c r="E28" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="5:15">
       <c r="E29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="5:15">
       <c r="E30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="5:15">
       <c r="E31" s="1" t="s">
         <v>1</v>
       </c>
@@ -2474,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="5:15">
       <c r="E32" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>